<commit_message>
Indications concernant le problème de transport 2
</commit_message>
<xml_diff>
--- a/26. Recherche opérationelle en Excel/12 - MULTIPLE- EXCELLENT FICHIER AVEC TRANSPORT,SAC A DOS,/Distribution et logistique - Examples multiples .xlsx
+++ b/26. Recherche opérationelle en Excel/12 - MULTIPLE- EXCELLENT FICHIER AVEC TRANSPORT,SAC A DOS,/Distribution et logistique - Examples multiples .xlsx
@@ -644,7 +644,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="275">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1527,6 +1527,15 @@
   <si>
     <t>Total products shipped out of usine 2</t>
   </si>
+  <si>
+    <t xml:space="preserve">ASPECT DE LA FUNCTION OBJECTIF DANS EXCEL </t>
+  </si>
+  <si>
+    <t>=SUMPRODUCT(B10:E11;B25:E26)+SUMPRODUCT(B14:F15;B31:F32)+SUMPRODUCT(B18:F21;B37:F40)</t>
+  </si>
+  <si>
+    <t>ON RETROUVE LES NOMS DES GROUPES DE CELLULES SOUS LONGLET FORMULAT DANS NAME MANAGER</t>
+  </si>
 </sst>
 </file>
 
@@ -1536,7 +1545,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -1610,8 +1619,13 @@
       <color theme="1"/>
       <name val="MS Sans Serif"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="MS Sans Serif"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1691,6 +1705,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2755,7 +2775,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="330">
+  <cellXfs count="332">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3522,6 +3542,8 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="95" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="93" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="94" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5025,7 +5047,7 @@
   <dimension ref="A1:U73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="S61" sqref="S61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="12.6"/>
@@ -6540,6 +6562,19 @@
       <c r="F56" s="254"/>
       <c r="G56" s="254"/>
       <c r="H56" s="255"/>
+      <c r="K56" s="330" t="s">
+        <v>272</v>
+      </c>
+      <c r="L56" s="330"/>
+      <c r="M56" s="330"/>
+      <c r="N56" s="330"/>
+      <c r="O56" s="330"/>
+      <c r="P56" s="330"/>
+      <c r="Q56" s="330"/>
+      <c r="R56" s="330"/>
+      <c r="S56" s="330"/>
+      <c r="T56" s="330"/>
+      <c r="U56" s="330"/>
     </row>
     <row r="57" spans="1:21">
       <c r="A57" s="259" t="s">
@@ -6552,6 +6587,19 @@
       <c r="F57" s="254"/>
       <c r="G57" s="254"/>
       <c r="H57" s="255"/>
+      <c r="K57" s="331" t="s">
+        <v>273</v>
+      </c>
+      <c r="L57" s="330"/>
+      <c r="M57" s="330"/>
+      <c r="N57" s="330"/>
+      <c r="O57" s="330"/>
+      <c r="P57" s="330"/>
+      <c r="Q57" s="330"/>
+      <c r="R57" s="330"/>
+      <c r="S57" s="330"/>
+      <c r="T57" s="330"/>
+      <c r="U57" s="330"/>
     </row>
     <row r="58" spans="1:21">
       <c r="A58" s="259"/>
@@ -6564,6 +6612,17 @@
       <c r="F58" s="254"/>
       <c r="G58" s="254"/>
       <c r="H58" s="255"/>
+      <c r="K58" s="330"/>
+      <c r="L58" s="330"/>
+      <c r="M58" s="330"/>
+      <c r="N58" s="330"/>
+      <c r="O58" s="330"/>
+      <c r="P58" s="330"/>
+      <c r="Q58" s="330"/>
+      <c r="R58" s="330"/>
+      <c r="S58" s="330"/>
+      <c r="T58" s="330"/>
+      <c r="U58" s="330"/>
     </row>
     <row r="59" spans="1:21">
       <c r="A59" s="259"/>
@@ -6576,6 +6635,19 @@
       <c r="F59" s="254"/>
       <c r="G59" s="254"/>
       <c r="H59" s="255"/>
+      <c r="K59" s="330" t="s">
+        <v>274</v>
+      </c>
+      <c r="L59" s="330"/>
+      <c r="M59" s="330"/>
+      <c r="N59" s="330"/>
+      <c r="O59" s="330"/>
+      <c r="P59" s="330"/>
+      <c r="Q59" s="330"/>
+      <c r="R59" s="330"/>
+      <c r="S59" s="330"/>
+      <c r="T59" s="330"/>
+      <c r="U59" s="330"/>
     </row>
     <row r="60" spans="1:21">
       <c r="A60" s="259"/>
@@ -6588,6 +6660,17 @@
       <c r="F60" s="254"/>
       <c r="G60" s="254"/>
       <c r="H60" s="255"/>
+      <c r="K60" s="330"/>
+      <c r="L60" s="330"/>
+      <c r="M60" s="330"/>
+      <c r="N60" s="330"/>
+      <c r="O60" s="330"/>
+      <c r="P60" s="330"/>
+      <c r="Q60" s="330"/>
+      <c r="R60" s="330"/>
+      <c r="S60" s="330"/>
+      <c r="T60" s="330"/>
+      <c r="U60" s="330"/>
     </row>
     <row r="61" spans="1:21">
       <c r="A61" s="259" t="s">
@@ -6600,6 +6683,17 @@
       <c r="F61" s="254"/>
       <c r="G61" s="254"/>
       <c r="H61" s="255"/>
+      <c r="K61" s="330"/>
+      <c r="L61" s="330"/>
+      <c r="M61" s="330"/>
+      <c r="N61" s="330"/>
+      <c r="O61" s="330"/>
+      <c r="P61" s="330"/>
+      <c r="Q61" s="330"/>
+      <c r="R61" s="330"/>
+      <c r="S61" s="330"/>
+      <c r="T61" s="330"/>
+      <c r="U61" s="330"/>
     </row>
     <row r="62" spans="1:21">
       <c r="A62" s="259"/>
@@ -6612,6 +6706,17 @@
       <c r="F62" s="254"/>
       <c r="G62" s="254"/>
       <c r="H62" s="255"/>
+      <c r="K62" s="330"/>
+      <c r="L62" s="330"/>
+      <c r="M62" s="330"/>
+      <c r="N62" s="330"/>
+      <c r="O62" s="330"/>
+      <c r="P62" s="330"/>
+      <c r="Q62" s="330"/>
+      <c r="R62" s="330"/>
+      <c r="S62" s="330"/>
+      <c r="T62" s="330"/>
+      <c r="U62" s="330"/>
     </row>
     <row r="63" spans="1:21">
       <c r="A63" s="259"/>
@@ -6624,6 +6729,17 @@
       <c r="F63" s="254"/>
       <c r="G63" s="254"/>
       <c r="H63" s="255"/>
+      <c r="K63" s="330"/>
+      <c r="L63" s="330"/>
+      <c r="M63" s="330"/>
+      <c r="N63" s="330"/>
+      <c r="O63" s="330"/>
+      <c r="P63" s="330"/>
+      <c r="Q63" s="330"/>
+      <c r="R63" s="330"/>
+      <c r="S63" s="330"/>
+      <c r="T63" s="330"/>
+      <c r="U63" s="330"/>
     </row>
     <row r="64" spans="1:21">
       <c r="A64" s="259"/>
@@ -6636,8 +6752,19 @@
       <c r="F64" s="254"/>
       <c r="G64" s="254"/>
       <c r="H64" s="255"/>
-    </row>
-    <row r="65" spans="1:8">
+      <c r="K64" s="330"/>
+      <c r="L64" s="330"/>
+      <c r="M64" s="330"/>
+      <c r="N64" s="330"/>
+      <c r="O64" s="330"/>
+      <c r="P64" s="330"/>
+      <c r="Q64" s="330"/>
+      <c r="R64" s="330"/>
+      <c r="S64" s="330"/>
+      <c r="T64" s="330"/>
+      <c r="U64" s="330"/>
+    </row>
+    <row r="65" spans="1:21">
       <c r="A65" s="259"/>
       <c r="B65" s="260" t="s">
         <v>62</v>
@@ -6648,8 +6775,19 @@
       <c r="F65" s="254"/>
       <c r="G65" s="254"/>
       <c r="H65" s="255"/>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="K65" s="330"/>
+      <c r="L65" s="330"/>
+      <c r="M65" s="330"/>
+      <c r="N65" s="330"/>
+      <c r="O65" s="330"/>
+      <c r="P65" s="330"/>
+      <c r="Q65" s="330"/>
+      <c r="R65" s="330"/>
+      <c r="S65" s="330"/>
+      <c r="T65" s="330"/>
+      <c r="U65" s="330"/>
+    </row>
+    <row r="66" spans="1:21">
       <c r="A66" s="259" t="s">
         <v>63</v>
       </c>
@@ -6660,8 +6798,19 @@
       <c r="F66" s="254"/>
       <c r="G66" s="254"/>
       <c r="H66" s="255"/>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="K66" s="330"/>
+      <c r="L66" s="330"/>
+      <c r="M66" s="330"/>
+      <c r="N66" s="330"/>
+      <c r="O66" s="330"/>
+      <c r="P66" s="330"/>
+      <c r="Q66" s="330"/>
+      <c r="R66" s="330"/>
+      <c r="S66" s="330"/>
+      <c r="T66" s="330"/>
+      <c r="U66" s="330"/>
+    </row>
+    <row r="67" spans="1:21">
       <c r="A67" s="259"/>
       <c r="B67" s="260"/>
       <c r="C67" s="254"/>
@@ -6670,8 +6819,19 @@
       <c r="F67" s="254"/>
       <c r="G67" s="254"/>
       <c r="H67" s="255"/>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="K67" s="330"/>
+      <c r="L67" s="330"/>
+      <c r="M67" s="330"/>
+      <c r="N67" s="330"/>
+      <c r="O67" s="330"/>
+      <c r="P67" s="330"/>
+      <c r="Q67" s="330"/>
+      <c r="R67" s="330"/>
+      <c r="S67" s="330"/>
+      <c r="T67" s="330"/>
+      <c r="U67" s="330"/>
+    </row>
+    <row r="68" spans="1:21">
       <c r="A68" s="264" t="s">
         <v>31</v>
       </c>
@@ -6682,8 +6842,19 @@
       <c r="F68" s="254"/>
       <c r="G68" s="254"/>
       <c r="H68" s="255"/>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="K68" s="330"/>
+      <c r="L68" s="330"/>
+      <c r="M68" s="330"/>
+      <c r="N68" s="330"/>
+      <c r="O68" s="330"/>
+      <c r="P68" s="330"/>
+      <c r="Q68" s="330"/>
+      <c r="R68" s="330"/>
+      <c r="S68" s="330"/>
+      <c r="T68" s="330"/>
+      <c r="U68" s="330"/>
+    </row>
+    <row r="69" spans="1:21">
       <c r="A69" s="259" t="s">
         <v>64</v>
       </c>
@@ -6695,7 +6866,7 @@
       <c r="G69" s="254"/>
       <c r="H69" s="255"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:21">
       <c r="A70" s="259" t="s">
         <v>65</v>
       </c>
@@ -6707,7 +6878,7 @@
       <c r="G70" s="254"/>
       <c r="H70" s="255"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:21">
       <c r="A71" s="259" t="s">
         <v>66</v>
       </c>
@@ -6719,7 +6890,7 @@
       <c r="G71" s="254"/>
       <c r="H71" s="255"/>
     </row>
-    <row r="72" spans="1:8" ht="13.2" thickBot="1">
+    <row r="72" spans="1:21" ht="13.2" thickBot="1">
       <c r="A72" s="261" t="s">
         <v>67</v>
       </c>
@@ -6731,7 +6902,7 @@
       <c r="G72" s="256"/>
       <c r="H72" s="257"/>
     </row>
-    <row r="73" spans="1:8" ht="13.2" thickTop="1"/>
+    <row r="73" spans="1:21" ht="13.2" thickTop="1"/>
   </sheetData>
   <printOptions gridLinesSet="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>